<commit_message>
Now blancoValueObjectKt is implemented.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectPhpSimpleSample.xlsx
+++ b/meta/objects/BlancoValueObjectPhpSimpleSample.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObject/meta/objects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E84445BC-ADD0-094E-8E1F-A1567B5E3523}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D3886F-2793-B644-B4FD-FA9E831300E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5000" yWindow="2960" windowWidth="21680" windowHeight="11800" tabRatio="640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5000" yWindow="2960" windowWidth="21680" windowHeight="11800" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
     <sheet name="config" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <definedNames>
     <definedName name="accessScope">config!$B$4:$B$6</definedName>
     <definedName name="accessScope2">config!$B$4:$B$5</definedName>
@@ -103,10 +100,6 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>blanco.sample.valueobject</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
     <t>バリューオブジェクトのサンプル。このクラスは単にサンプルです。実際の動作には利用されません。</t>
     <phoneticPr fontId="4"/>
   </si>
@@ -220,6 +213,10 @@
   <si>
     <t>○</t>
     <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>blanco.sample.valueobjectkt</t>
+    <phoneticPr fontId="4"/>
   </si>
 </sst>
 </file>
@@ -751,12 +748,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -785,6 +776,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -869,21 +866,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="valueObject"/>
-      <sheetName val="config"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1213,8 +1195,8 @@
   </sheetPr>
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1261,7 +1243,7 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="8"/>
@@ -1273,7 +1255,7 @@
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="10" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="D7" s="39"/>
       <c r="E7" s="11"/>
@@ -1285,7 +1267,7 @@
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
@@ -1308,12 +1290,12 @@
       <c r="H9" s="8"/>
     </row>
     <row r="10" spans="1:10" s="34" customFormat="1">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="41"/>
+      <c r="C10" s="42" t="s">
         <v>27</v>
-      </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="44" t="s">
-        <v>28</v>
       </c>
       <c r="D10"/>
       <c r="E10"/>
@@ -1321,12 +1303,12 @@
       <c r="G10"/>
     </row>
     <row r="11" spans="1:10" s="34" customFormat="1">
-      <c r="A11" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="43"/>
-      <c r="C11" s="44" t="s">
+      <c r="A11" s="40" t="s">
         <v>28</v>
+      </c>
+      <c r="B11" s="41"/>
+      <c r="C11" s="42" t="s">
+        <v>27</v>
       </c>
       <c r="D11"/>
       <c r="E11"/>
@@ -1344,7 +1326,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="32"/>
       <c r="C13" s="32"/>
@@ -1394,37 +1376,37 @@
       <c r="J16" s="15"/>
     </row>
     <row r="17" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="40" t="s">
+      <c r="C17" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17" s="40" t="s">
+      <c r="D17" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="40" t="s">
+      <c r="F17" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="G17" s="40"/>
+      <c r="G17" s="51"/>
       <c r="H17" s="16"/>
       <c r="I17" s="17"/>
       <c r="J17" s="9"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="41"/>
-      <c r="B18" s="41"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
+      <c r="A18" s="52"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
       <c r="H18" s="18"/>
       <c r="I18" s="30"/>
       <c r="J18" s="15"/>
@@ -1434,17 +1416,17 @@
         <v>1</v>
       </c>
       <c r="B19" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="21" t="s">
         <v>18</v>
-      </c>
-      <c r="C19" s="21" t="s">
-        <v>19</v>
       </c>
       <c r="D19" s="21"/>
       <c r="E19" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>
@@ -1456,15 +1438,15 @@
         <v>2</v>
       </c>
       <c r="B20" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="21" t="s">
         <v>21</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>22</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="21"/>
       <c r="F20" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G20" s="22"/>
       <c r="H20" s="22"/>
@@ -1517,7 +1499,7 @@
     <mergeCell ref="D17:D18"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
-  <dataValidations disablePrompts="1" count="3">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E39" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
@@ -1544,7 +1526,7 @@
   </sheetPr>
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
@@ -1560,65 +1542,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="46" t="s">
+      <c r="M1" s="44"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="B3" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="46"/>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="B3" s="47" t="s">
+      <c r="D3" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="F3" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="47" t="s">
+      <c r="H3" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="47" t="s">
+      <c r="J3" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="47" t="s">
+    </row>
+    <row r="4" spans="1:13">
+      <c r="B4" s="46"/>
+      <c r="D4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="J4" s="47"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="B5" s="48" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="B4" s="48"/>
-      <c r="D4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="J4" s="49"/>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="B5" s="50" t="s">
+      <c r="D5" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="J5" s="51" t="s">
-        <v>38</v>
+      <c r="F5" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="49" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="B6" s="52"/>
+      <c r="B6" s="50"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4"/>

</xml_diff>

<commit_message>
CanDo:  * read php style definition sheets and output typescript codes. ToDo:  * Search classes from parsed meta files in same time, and create import automatically.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectPhpSimpleSample.xlsx
+++ b/meta/objects/BlancoValueObjectPhpSimpleSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/objects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectTs/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D3886F-2793-B644-B4FD-FA9E831300E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F602A22-9546-B449-81CE-E1EEB7D67EA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5000" yWindow="2960" windowWidth="21680" windowHeight="11800" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -215,7 +215,7 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>blanco.sample.valueobjectkt</t>
+    <t>blanco.sample.valueobjectts</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1195,8 +1195,8 @@
   </sheetPr>
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>

</xml_diff>

<commit_message>
0.0.6: fix bugs on Nullable handling. * TypeScript should have default value but nullable or interfaces.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectPhpSimpleSample.xlsx
+++ b/meta/objects/BlancoValueObjectPhpSimpleSample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectTs/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F602A22-9546-B449-81CE-E1EEB7D67EA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9573E5-9902-AD4B-82F3-FA08086FA65C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5000" yWindow="2960" windowWidth="21680" windowHeight="11800" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9100" yWindow="6000" windowWidth="21680" windowHeight="11800" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -41,12 +41,12 @@
     <definedName name="必須" localSheetId="1">#REF!</definedName>
     <definedName name="必須">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>クラス名</t>
   </si>
@@ -216,6 +216,14 @@
   </si>
   <si>
     <t>blanco.sample.valueobjectts</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Nullable</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>○</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -300,7 +308,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -681,11 +689,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -781,6 +815,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1193,42 +1235,42 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
-    <col min="2" max="5" width="23.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="28" style="1" customWidth="1"/>
-    <col min="9" max="9" width="33.33203125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="1"/>
+    <col min="2" max="6" width="23.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="28" style="1" customWidth="1"/>
+    <col min="10" max="10" width="33.33203125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19">
+    <row r="1" spans="1:11" ht="19">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -1236,8 +1278,9 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="F5" s="53"/>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1247,9 +1290,10 @@
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="9"/>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="F6" s="54"/>
+      <c r="G6" s="9"/>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -1259,9 +1303,10 @@
       </c>
       <c r="D7" s="39"/>
       <c r="E7" s="11"/>
-      <c r="F7" s="9"/>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="F7" s="54"/>
+      <c r="G7" s="9"/>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -1273,9 +1318,10 @@
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
-      <c r="H8" s="8"/>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="H8" s="12"/>
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -1287,9 +1333,10 @@
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="10" spans="1:10" s="34" customFormat="1">
+      <c r="H9" s="12"/>
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="1:11" s="34" customFormat="1">
       <c r="A10" s="40" t="s">
         <v>26</v>
       </c>
@@ -1301,21 +1348,23 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10"/>
-    </row>
-    <row r="11" spans="1:10" s="34" customFormat="1">
+      <c r="H10"/>
+    </row>
+    <row r="11" spans="1:11" s="34" customFormat="1">
       <c r="A11" s="40" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="41"/>
       <c r="C11" s="42" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="D11"/>
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11"/>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="H11"/>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
@@ -1323,8 +1372,9 @@
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="H12" s="13"/>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="31" t="s">
         <v>19</v>
       </c>
@@ -1332,13 +1382,14 @@
       <c r="C13" s="32"/>
       <c r="D13" s="32"/>
       <c r="E13" s="32"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="34"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="33"/>
       <c r="H13" s="34"/>
       <c r="I13" s="34"/>
       <c r="J13" s="34"/>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="K13" s="34"/>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="35" t="s">
         <v>0</v>
       </c>
@@ -1346,13 +1397,14 @@
       <c r="C14" s="37"/>
       <c r="D14" s="37"/>
       <c r="E14" s="37"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="34"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="38"/>
       <c r="H14" s="34"/>
       <c r="I14" s="34"/>
       <c r="J14" s="34"/>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="K14" s="34"/>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="13"/>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
@@ -1360,8 +1412,9 @@
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="H15" s="13"/>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
@@ -1372,10 +1425,11 @@
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="15"/>
-    </row>
-    <row r="17" spans="1:10" ht="13.5" customHeight="1">
+      <c r="I16" s="14"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="15"/>
+    </row>
+    <row r="17" spans="1:11" ht="13.5" customHeight="1">
       <c r="A17" s="52" t="s">
         <v>4</v>
       </c>
@@ -1391,27 +1445,31 @@
       <c r="E17" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="51" t="s">
+      <c r="F17" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="G17" s="51"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="9"/>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="H17" s="51"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="9"/>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="52"/>
       <c r="B18" s="52"/>
       <c r="C18" s="51"/>
       <c r="D18" s="51"/>
       <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
+      <c r="F18" s="56"/>
       <c r="G18" s="51"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="15"/>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="H18" s="51"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="15"/>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="19">
         <v>1</v>
       </c>
@@ -1425,15 +1483,16 @@
       <c r="E19" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="21" t="s">
+      <c r="F19" s="21"/>
+      <c r="G19" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G19" s="22"/>
       <c r="H19" s="22"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="15"/>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="I19" s="22"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="15"/>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="19">
         <v>2</v>
       </c>
@@ -1446,61 +1505,68 @@
       <c r="D20" s="21"/>
       <c r="E20" s="21"/>
       <c r="F20" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="G20" s="22"/>
       <c r="H20" s="22"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="15"/>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="I20" s="22"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="15"/>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="19"/>
       <c r="B21" s="20"/>
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
       <c r="E21" s="21"/>
       <c r="F21" s="21"/>
-      <c r="G21" s="22"/>
+      <c r="G21" s="21"/>
       <c r="H21" s="22"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="15"/>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="I21" s="22"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="15"/>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="19"/>
       <c r="B22" s="20"/>
       <c r="C22" s="21"/>
       <c r="D22" s="21"/>
       <c r="E22" s="21"/>
       <c r="F22" s="21"/>
-      <c r="G22" s="22"/>
+      <c r="G22" s="21"/>
       <c r="H22" s="22"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="15"/>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="I22" s="22"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="15"/>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="24"/>
       <c r="B23" s="25"/>
       <c r="C23" s="26"/>
       <c r="D23" s="26"/>
       <c r="E23" s="26"/>
       <c r="F23" s="26"/>
-      <c r="G23" s="27"/>
+      <c r="G23" s="26"/>
       <c r="H23" s="27"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="15"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="F17:G18"/>
+  <mergeCells count="7">
+    <mergeCell ref="G17:H18"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="E17:E18"/>
     <mergeCell ref="D17:D18"/>
+    <mergeCell ref="F17:F18"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E39" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E39:F39" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>